<commit_message>
testing excel parsing, uploads and report generation
</commit_message>
<xml_diff>
--- a/uploads/student_data5.xlsx
+++ b/uploads/student_data5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marks.r\Documents\REPORT_WRITING_APPLICATION\Batch_Report\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6BE46E-91EE-476D-81DB-E82F77672E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45817543-226E-4B60-81AF-57061935332C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA61B80E-0392-4D06-90DD-9D43CDF00CCC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>student_name</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>It has been a pleasure having Ryan in 11A. He is a lovely and well-mannered young man who demonstrates humility, kindness, and sensitivity to the needs of others. He has found the transition to Year 9 positive but some subjects and their increase in workload challenging. He should recognise the tremendous effort he has shown this year, and the diligence and hard work he has invested in his classes. Perhaps Ryan could consider subjects that he might find more interest and stimulation in. It is great to see that he has embraced many of the extra-curricular opportunities at the College and sees these as an opportunity for healthy competition and connect with community. Ryan has participated in the House Cross Country, Athletics, and the Swimming Carnival as well as Musiquest, String Ensemble and Chapel Band. He also really enjoyed the Senior Rally Day and helped to run the class fundraiser. Ryan has expressed commitment to Church and Youth, prayer and worship and I encourage him to continue to place his trust in God. It is a delight having Ryan in Home Group and I hope he has a restful holiday break and prospers in the year ahead</t>
+  </si>
+  <si>
+    <t>adjectives</t>
+  </si>
+  <si>
+    <t>kind thoughtful</t>
   </si>
 </sst>
 </file>
@@ -467,24 +473,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B70A5B5-45BB-4225-8A4B-0CDB29467C86}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3:XFD4"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="186.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="158.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="118.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="186.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="158.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="118.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,19 +502,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -518,18 +528,21 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
testing user upload and report generation flow
</commit_message>
<xml_diff>
--- a/uploads/student_data5.xlsx
+++ b/uploads/student_data5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marks.r\Documents\REPORT_WRITING_APPLICATION\Batch_Report\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45817543-226E-4B60-81AF-57061935332C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888E6E26-AA42-4924-B8AC-789A8D5C9A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA61B80E-0392-4D06-90DD-9D43CDF00CCC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>student_name</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cooper </t>
-  </si>
-  <si>
-    <t>9D</t>
   </si>
   <si>
     <t>male</t>
@@ -477,7 +474,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E6" sqref="E6"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +499,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -521,26 +518,26 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="I2" s="1"/>
     </row>

</xml_diff>